<commit_message>
got jobType for datascrape to work
</commit_message>
<xml_diff>
--- a/Workflows/P2-WorkflowForZipRecruiter/exceltestsheet/ZipRecruiterData.xlsx
+++ b/Workflows/P2-WorkflowForZipRecruiter/exceltestsheet/ZipRecruiterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Projects\Goldeneyez-P2\Goldeneyez-P2\Workflows\P2-WorkflowForZipRecruiter\exceltestsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA34354-CE29-453D-A6A8-72623AAD58BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F520D665-F928-46B3-9202-0BB5E3A13998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="0" activeTab="0" xr2:uid="{2293894A-00AC-4E8F-B2D5-30D97C5CB308}"/>
   </x:bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <x:si>
     <x:t>jobTitle</x:t>
   </x:si>
@@ -46,6 +46,9 @@
     <x:t>jobLocation</x:t>
   </x:si>
   <x:si>
+    <x:t>jobType</x:t>
+  </x:si>
+  <x:si>
     <x:t>jobDescription</x:t>
   </x:si>
   <x:si>
@@ -61,10 +64,13 @@
     <x:t>San Francisco, CA</x:t>
   </x:si>
   <x:si>
+    <x:t>Full-Time</x:t>
+  </x:si>
+  <x:si>
     <x:t>Key areas of responsibility include providing end-user support for Windows Desktop OS (v7/v10), Office 365, PC Imaging and general IT support. * Additionally, the successful candidate will also ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/k/l/AALi-w3Z4jdQfTbeqlVGie96q6iNGp26x_WwHpDDl9bcOxHt21wqWr1CAHn3zgJWJZTOPKM7tuvl3UEKVbP1zRG3LxS2Vrw4hu60dPgrw3HuMDQrUNAZ46KkK9R1tEM6rdlELbXvOBruufKzzLSwRxqVQIy0oPGFhvot3syiJPbLbaWQZFfZKQ</x:t>
+    <x:t>https://www.ziprecruiter.com/k/l/AAI2l2wIvxwZuK69KBsnehmx15x7C8P9ZhOtRKx1wiZhFq9I2g5zVvUMnkb2SUcGaoidZJHRIsbukdjyHcrmUlaSTQZqIp6RxdcVYiv_CaUJbYbRkTa3le9xAVdVMgAieMZU5z4cNZPfvX2k3_iV7NG2mOp3lpSiP-ZPbiBLMfnfIzcDdP-E3g</x:t>
   </x:si>
   <x:si>
     <x:t>Electrical Design Engineer</x:t>
@@ -73,25 +79,25 @@
     <x:t>CyberCoders</x:t>
   </x:si>
   <x:si>
+    <x:t>Technician will disassemble unit and examine condition, movement, or alignment of parts visually or using gauges. The technician will replace defective parts using hand tools, arbor press, flexible ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.ziprecruiter.com/k/l/AAJf5K74lQVBJoajhRhRXr5Dkoo16PXUSB_5vom7iuyodw6tq1XCh3WLusLVgedDuaJzLGa6sDZLRPqwVY60TynCd9YZ4iN7Ko9CBJFCjMUXIjguWfy4VP1OCJKmici77KwfMWFIwsm5zh2SciS257NipaZ-m5uZD_xJbcN_OeRW1ivpkJjsSg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Design Engineer (ESC) - Electrical - San Ramon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PG&amp;E Corporation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>San Ramon, CA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Watch A Day in the Life of a Crown Field Service Technician! click here For a limited time choose your Incentive! For a limited time new hires will have the option to pick 1 of the 3 incentives * 2 ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/k/l/AAJ3USObVO-nazjpahjvgvpU8XMMqjpYpZ8VUPS-Y78a9i_CqhanWy7zKsjSLTQUG_PgyJKpNn-5vbzYX1as8KK04y9jOs6P8kiK9szo9bMsFHlaDbB0xHBEkHMjVHzaRggLXIwkOXsuHt1VUDSp4HJ7gVMk4ucOO0r79vhQbD9RbY9aUg3oRQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Design Engineer (ESC) - Electrical - San Ramon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PG&amp;E Corporation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>San Ramon, CA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>We are seeking a Help Desk Technician to join our team! You will be supporting one of the largest, most collaborative enterprise service desks in the United States defense space. As a service desk ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AAJTP78DFf_7tA43gIcMWLia2BndJvvnsB8OC-xKnjVL-i6TvLEgo4gTrb0JakRN6793a5KsqNdTvETIeripWGViAomvuZkpPEdGRe5c0nLML2Ea3qy4h98zUqm8hrEXH6FDQlAtTUTFtVJ6FaD33OD79BlUdXIxVg2ayNlNibEAynScZjRgBQ</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AAL3PwFI-Zy48BR4UMmv7fPMuhcEalERCiZ_OAvQhMZBZo_TXNxt48kTGg10CFjAOhoZW29RzbfpKcMdy0B1lRumiznVQ96JHIUbtZSq0NMnSsNrWNuQTXuUvBGptguA3NKmKHGBW3lFl8uFYyM7bAy0YGsPNAVKZBNLAgABSUpsG63VhsrwDQ</x:t>
   </x:si>
   <x:si>
     <x:t>Arup</x:t>
@@ -100,7 +106,7 @@
     <x:t>Field Service - Maintenance Technician A Field Service Technician (Service Engineer) contributes to the success of Productivity by keeping our customers' CNC machine tools running at peak operating ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AAKHipdiZOK1000SrACBRxvBjhxoakw8bQByDFqaYOh5jWd48T4WaehyPcP96hlh1sv9fQWUWepW7K6Keh9VOP7-HPij6S2qw_Y14X_jCTqZXGueFrm_o0_yBrbtKkki1QElsPHbma3tknR3DR6x5HaCzR1u3X1gSCFHuCbBzrwgQvuBMFwd_w</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AAKNtzLM9LrKL3P4yw8qoYCxHPPjRcTAXtMjNdbHWf69ZRXHm13l5Ku6KpdHxAo1TKAbW9lfpCzWOFZioQNtqbhbh__90FagcZDxwexqrNNV_lXcnsPsH8braIyy7KByLqHRgaBUT17dKpPsAHaFHerAlKIc8mMNnPLPhzBwQHEa0uUmMeBN1w</x:t>
   </x:si>
   <x:si>
     <x:t>Electrical Engineer III</x:t>
@@ -115,64 +121,61 @@
     <x:t>Help Desk Technician Company: Ascend Staffing Reports To: CIO Pay: $15 - $16 + monthly bonus Job Summary IT Associate will provide technical support for Ascend Staffing's internal users, and assist ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AAJ9Xe_JVgHltFkp_0qYSvYWro3EGVKOiezhbkrXSHscrRnbyjg5t6PF7Pp09cS1ocavYayCG4VDZgZKnvstUEd1sc8-851YtSMleyO98lU8IkZ-W7PRcVbfxEHeAvMB2aSDmhAOY7ftB6TEZ0PBLozt0pIsqzv0fjt3M7oDwhPl9XUQobqQhw</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AAJvnnWTF5q5UV2fEelUCVy1ODYP57krvd0KmrwYz2gPJoWd_J9i35HZppKHgej5NbVs66ZGv3nRAWg2Jrahh9oouL_C-XBaTzd_A_rDDy4wv5qKwo_yvTHEs-XsxV5cR0-Va9s_V8Et6tWtzI7umxiPVyfr901NkK7HRfdtq-cs_ARWdSwJFg</x:t>
   </x:si>
   <x:si>
     <x:t>Electrical Engineer, Facebook Reality Labs</x:t>
   </x:si>
   <x:si>
-    <x:t>Facebook</x:t>
+    <x:t>Meta</x:t>
   </x:si>
   <x:si>
     <x:t>***This position requires commute to our offices. It is our clients that are remote.*** ***COVID vaccination is required to be considered for this position.*** Duties and Responsibilities * Be able to ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AAIB5ovbl447_FRwuwXuolITuYKJmP6ltNOE7Gq-j57JMR1DomXno0p8Z66jgMWjlu_a8QRZtlMk5xXLJmjHtyCwkM5fyQNqaBp8L4sufF7fCKO1AjwEKKreLpcnZchjg01u03JGtTwRLesHwA9pu3KoUf4gFMIme_d8KGuNbE_LIgnPptc0Eg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Research Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Mom Project</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AAK3f6V2vpS4qORP0KzXsgL5BHJ5FWYz7zQ3Q3-mh5RWIMHx39uUhSIRRWM9GSNsoI026pE5ScX75o3s8w3cPR5xHldsWY0GuhrLhmxq9nxXzhRxhEY5vOa6tFGKhuhghpfcjvVcQ4FH8ScV10jaQF7FvlctEg2DmqvHJu8Jxa_h6kOwaDdqeg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior .NET Developer (Remote)</x:t>
   </x:si>
   <x:si>
     <x:t>We are seeking an outgoing, eager to learn, tier 1 Support Technician to join our team ... Customer/End user desktop/laptop computers and related equipment (I.E. Hard drives, keyboard, mice ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/k/l/AALNOAzZGxQ5ZQ0Kw3hoLFwuD1T3tJLp0JsZUHNCGDKo9s7V7b1Y0Wpek7VLqscYZHgbXeqRRYQwQFAuEeVXGI9J1pu4ELX4q-Zll_W98d26o5AgY7GCmgstI7YrPAj3W2eSy0CWxoId2QYXxYk1pglkjOh_aV5KbJd1z9bOCTCqxWN0OxzufQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Construction Superintendent - Commercial Solar Projects</x:t>
+    <x:t>https://www.ziprecruiter.com/k/l/AAIVvNecE8xO1fRPT2P_6S-vQudrwZJZk1CyalGm0HJDQiNHMu4ggQclzd3ar1T1W6S3pJHHAMbsKH5H5-iQBFOHK-KUz8RV1eJPl1BC8JYLPNhjsVrr_LI5jq1VurFq9loVReMSTBQkdKMXrdfO3Rwm2e-airxJtCU08CI2_A3P9obX66OhYg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Expert, Advising Electrical Engineer - San Ramon</x:t>
   </x:si>
   <x:si>
     <x:t>POSITION PURPOSE: This position ensures that Reddy Ice field service equipment is well-maintained and functioning properly. DUTIES AND RESPONSIBILITIES: 1. Conducts repairs, service, installations ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/k/l/AAI5rl21O2kny9wovO7vNM8d3Bcz-C_YiZcPaJEDH6PBGlMinUGIV2nKGR-RBP_bPcmdcwqE_OJnXNCfVdp-ohFX997ZDsUrf6ZbCo7yXiW5yWV4m0H5gzx41UgohwNgLnhkv-ZTm5PYcGHX88sZ4gvQCKIh2ZGCDViSf6uqkBY0pxkQA_fZCg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Expert, Advising Electrical Engineer - San Ramon</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AAJ3lqOXag2XEGRLjwHNaVFmwccbhc6olq_Pvk2cOCwt8mSHS5eI_ikQQW3gHidT3BqLvFwSHtKgiFlwtmCtowJJlWeyBnEfJUnK11G6O3bVvDJwRNpQTrASkiumPeRcYHtIwx2Vb5DSVMCnhY26-sPE1lyRIKFjwiw-3wvpis95Hii0xVDDaQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Electrical Engineering Writer | PCB Design &amp; Manufacturing (Full-Time, Remote)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First Page Sage, LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Berkeley, CA</x:t>
   </x:si>
   <x:si>
     <x:t>Check out our video to experience a day in the life of a DISH Technician: The In-Home Services organization supports thousands of talented employees in 125+ facilities delivering service solutions to ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AAI1BsW5gko6xUe89CMH5GBq9lHSbHPkIKnjHQYqpCYg3MxHtmyFwZI6QfTmh-aCnNy3TY-AnxQRy7wIKCrvnoQN4LfQru46UN4Ryess2xCfAAg44tBEHNC0iE-PZl7rEJtMsrzHalLAoE7Qgad6F5lSkziZiaRyl-YQueT8EZtiErt60UPfGg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Electrical Engineering Writer | PCB Design &amp; Manufacturing (Full-Time, Remote)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>First Page Sage, LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Berkeley, CA</x:t>
+    <x:t>https://www.ziprecruiter.com/ek/l/AALiaqAWHTRwjQzyDmo8AZiCmZkQKIEx2ZeyRz4n9JnSF40wWj5_DTHqwcfSFz9QenjL0ve9uLPq2Qy2AWDbfvBtCSD0oQgr2_8QDye6JL2xZG1FynrS0lQ9048bjD1H3RPv5SSGX_0WA8NRKDTVMjT3bXp8SmKZAJGpqwXgyp0jSgMh6vPiow</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MEMs Design Engineer</x:t>
   </x:si>
   <x:si>
     <x:t>Description Our team is seeking a qualified Level 1 service desk technicians to support one of the largest, most collaborative enterprise service desks in the defense space. Under the Global Service ...</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.ziprecruiter.com/ek/l/AALMo0Vkht8cXb-qnAFkPYHymwS_LBJMJtway46HyYw4-2DN_5mIO4vhhgmacaBSObr0-EKG9tgPodGRw01Z1q6igk2UzDKYw7WLV0Wb_PXVt8ETPs37RaA-vvjJmB4cgLaVGMdrKOu_r3_NJJaYF7vwvVVF311BtsahONYAoDURw-wPSZZCGxA</x:t>
+    <x:t>https://www.ziprecruiter.com/k/l/AAIAO7ZPCl2NrJt_CTKpzwJ3KrUBMH-wIhv2QS5gb89Kht7N5iQRaeTTrHj-Ta3vrbsHwZaKs6AsDsOd5trh4DeZjDFzHjPmWYoJx-MJikRNCX6NvHR2xwRV1XYkc-AIOBoxZ4mpnypcCvq30i42tkgX3Y0fUbxwkW0LyvYacaqUrVSUOO5RJfM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -215,8 +218,20 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="22">
+  <x:cellStyleXfs count="26">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -614,10 +629,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E11"/>
+  <x:dimension ref="A1:F11"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G3" sqref="G3 G3:G3"/>
+      <x:selection activeCell="F1" sqref="F1 F1:F1 F1:F1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,10 +640,12 @@
     <x:col min="1" max="1" width="52" style="4" customWidth="1"/>
     <x:col min="2" max="2" width="19.855469" style="4" customWidth="1"/>
     <x:col min="3" max="3" width="29" style="4" customWidth="1"/>
-    <x:col min="4" max="4" width="34.855469" style="5" customWidth="1"/>
+    <x:col min="4" max="4" width="11.140625" style="4" customWidth="1"/>
+    <x:col min="5" max="5" width="34.140625" style="5" customWidth="1"/>
+    <x:col min="6" max="6" width="59.140625" style="5" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -638,181 +655,214 @@
       <x:c r="C1" s="4" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="5" t="s">
+      <x:c r="D1" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="4" t="s">
+      <x:c r="E1" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="F1" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A2" s="4" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="4" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="5" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D3" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F3" s="5" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B4" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C4" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D4" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E4" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F4" s="5" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="s">
+      <x:c r="B5" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C5" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D5" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E5" s="5" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F5" s="5" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B6" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C6" s="4" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D6" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F6" s="5" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="4" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B7" s="4" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C7" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D7" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E7" s="5" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F7" s="5" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="4" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B8" s="4" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="5" t="s">
+      <x:c r="C8" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E2" s="4" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="4" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B3" s="4" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C3" s="4" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D3" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E3" s="4" t="s">
+      <x:c r="D8" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="5" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F8" s="5" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="4" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B9" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C9" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D9" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E9" s="5" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F9" s="5" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="4" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B10" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C10" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D10" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E10" s="5" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="F10" s="5" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="4" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B11" s="4" t="s">
         <x:v>13</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="4" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B4" s="4" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C4" s="4" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D4" s="5" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E4" s="4" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B5" s="4" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C5" s="4" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D5" s="5" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E5" s="4" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="4" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B6" s="4" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C6" s="4" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="D6" s="5" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E6" s="4" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="4" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="B7" s="4" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C7" s="4" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D7" s="5" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E7" s="4" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="4" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B8" s="4" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C8" s="4" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D8" s="5" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="E8" s="4" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="4" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="B9" s="4" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C9" s="4" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D9" s="5" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="E9" s="4" t="s">
-        <x:v>37</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="4" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="B10" s="4" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C10" s="4" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D10" s="5" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="E10" s="4" t="s">
-        <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:7" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="4" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="B11" s="4" t="s">
-        <x:v>42</x:v>
-      </x:c>
       <x:c r="C11" s="4" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="D11" s="5" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="E11" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D11" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E11" s="5" t="s">
         <x:v>45</x:v>
+      </x:c>
+      <x:c r="F11" s="5" t="s">
+        <x:v>46</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>